<commit_message>
Add Lab4 tests, add Coverage Reports. Modify excel file.
</commit_message>
<xml_diff>
--- a/Docs/Lab4/Lab04_WBT_TCs_Form.xlsx
+++ b/Docs/Lab4/Lab04_WBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE25199D-359C-4C51-B952-5B04388CEA89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B56C9-37F9-4A3A-827F-EEC9EBE8BA81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Statistics</t>
-  </si>
-  <si>
-    <t>&lt;coverage percent&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Covered source code </t>
@@ -428,6 +425,9 @@
   </si>
   <si>
     <t>Employee Ionel a fost modificat</t>
+  </si>
+  <si>
+    <t>NullPointerException</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1122,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1151,9 +1151,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1225,6 +1222,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1252,48 +1270,114 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1303,10 +1387,13 @@
     <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1318,26 +1405,77 @@
     <xf numFmtId="49" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1351,152 +1489,11 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2819,12 +2816,12 @@
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
+      <c r="D1" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="L2" s="13" t="s">
@@ -2835,33 +2832,33 @@
       <c r="O2" s="13"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="50"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="56"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="L4" s="51" t="s">
+      <c r="L4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="20" t="s">
-        <v>58</v>
+      <c r="M4" s="57"/>
+      <c r="N4" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="48">
+      <c r="P4" s="54">
         <v>1211</v>
       </c>
-      <c r="Q4" s="50"/>
+      <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -2877,7 +2874,7 @@
     </row>
     <row r="8" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2930,545 +2927,551 @@
   </sheetPr>
   <dimension ref="B1:P38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2" style="24" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="65.109375" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="24" customWidth="1"/>
-    <col min="5" max="10" width="8.88671875" style="24"/>
-    <col min="11" max="11" width="53.88671875" style="24" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" style="24" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="57.44140625" style="24" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="24"/>
+    <col min="1" max="1" width="2" style="23" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.109375" style="23" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="23" customWidth="1"/>
+    <col min="5" max="10" width="8.88671875" style="23"/>
+    <col min="11" max="11" width="53.88671875" style="23" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" style="23" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57.44140625" style="23" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="23"/>
-      <c r="C1" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="54"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C2" s="25"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="58" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="59"/>
+      <c r="E5" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="E5" s="52" t="s">
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="M5" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="M5" s="67" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="101" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="23" t="s">
+      <c r="M7" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="72"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="27">
+        <v>1</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="N7" s="65"/>
-      <c r="O7" s="65"/>
-      <c r="P7" s="27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="28">
-        <v>1</v>
-      </c>
-      <c r="C8" s="100" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="65" t="s">
+      <c r="M8" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="65"/>
-      <c r="O8" s="65"/>
-      <c r="P8" s="27">
+      <c r="N8" s="72"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="26">
         <f>8-7+2</f>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="28">
+      <c r="B9" s="27">
         <v>2</v>
       </c>
-      <c r="C9" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="56"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="58"/>
-      <c r="M9" s="65" t="s">
+      <c r="C9" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="61"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="63"/>
+      <c r="M9" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="65" t="s">
+      <c r="N9" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="65"/>
-      <c r="P9" s="102">
+      <c r="O9" s="72"/>
+      <c r="P9" s="48">
         <f>3+1</f>
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="28">
+      <c r="B10" s="27">
         <v>3</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="64"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="66"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="27">
+        <v>4</v>
+      </c>
+      <c r="C11" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="61"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="28">
-        <v>4</v>
-      </c>
-      <c r="C11" s="45" t="s">
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="27">
+        <v>5</v>
+      </c>
+      <c r="C12" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="61"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="28">
-        <v>5</v>
-      </c>
-      <c r="C12" s="45" t="s">
+      <c r="E12" s="64"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="66"/>
+      <c r="M12" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="70"/>
+      <c r="O12" s="70"/>
+      <c r="P12" s="70"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="27">
+        <v>6</v>
+      </c>
+      <c r="C13" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="61"/>
-      <c r="M12" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="28">
-        <v>6</v>
-      </c>
-      <c r="C13" s="45" t="s">
+      <c r="E13" s="64"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="66"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="27">
+        <v>7</v>
+      </c>
+      <c r="C14" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="59"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="61"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="28">
-        <v>7</v>
-      </c>
-      <c r="C14" s="45" t="s">
+      <c r="E14" s="64"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="66"/>
+      <c r="M14" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="73"/>
+      <c r="P14" s="73"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="27">
+        <v>8</v>
+      </c>
+      <c r="C15" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="61"/>
-      <c r="M14" s="26" t="s">
+      <c r="E15" s="64"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="66"/>
+      <c r="M15" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" s="71"/>
+      <c r="P15" s="71"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="27">
+        <v>9</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="64"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="66"/>
+      <c r="M16" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="N16" s="71" t="s">
+        <v>71</v>
+      </c>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="27">
+        <v>10</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="66"/>
+      <c r="M17" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="27">
+        <v>11</v>
+      </c>
+      <c r="C18" s="44"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="66"/>
+      <c r="M18" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="N18" s="71" t="s">
+        <v>73</v>
+      </c>
+      <c r="O18" s="71"/>
+      <c r="P18" s="71"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="27">
+        <v>12</v>
+      </c>
+      <c r="C19" s="44"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="66"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="71"/>
+      <c r="O19" s="71"/>
+      <c r="P19" s="71"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="27">
+        <v>13</v>
+      </c>
+      <c r="C20" s="44"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="66"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="71"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="27">
+        <v>14</v>
+      </c>
+      <c r="C21" s="44"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="66"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="71"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B22" s="27">
+        <v>15</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="66"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="71"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B23" s="27">
+        <v>16</v>
+      </c>
+      <c r="C23" s="44"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
+      <c r="K23" s="66"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B24" s="27">
+        <v>17</v>
+      </c>
+      <c r="C24" s="44"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B25" s="27">
         <v>18</v>
       </c>
-      <c r="N14" s="66" t="s">
+      <c r="C25" s="44"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="66"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B26" s="27">
         <v>19</v>
       </c>
-      <c r="O14" s="66"/>
-      <c r="P14" s="66"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="28">
-        <v>8</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="61"/>
-      <c r="M15" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="N15" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="O15" s="55"/>
-      <c r="P15" s="55"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="28">
-        <v>9</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="61"/>
-      <c r="M16" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="N16" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="28">
-        <v>10</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="61"/>
-      <c r="M17" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="N17" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="O17" s="55"/>
-      <c r="P17" s="55"/>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="28">
-        <v>11</v>
-      </c>
-      <c r="C18" s="45"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="61"/>
-      <c r="M18" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="N18" s="55" t="s">
-        <v>74</v>
-      </c>
-      <c r="O18" s="55"/>
-      <c r="P18" s="55"/>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="28">
-        <v>12</v>
-      </c>
-      <c r="C19" s="45"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="61"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="28">
-        <v>13</v>
-      </c>
-      <c r="C20" s="45"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="61"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="55"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B21" s="28">
-        <v>14</v>
-      </c>
-      <c r="C21" s="45"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="61"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="28">
-        <v>15</v>
-      </c>
-      <c r="C22" s="45"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="61"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="55"/>
-      <c r="P22" s="55"/>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23" s="28">
-        <v>16</v>
-      </c>
-      <c r="C23" s="45"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="61"/>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B24" s="28">
-        <v>17</v>
-      </c>
-      <c r="C24" s="45"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="61"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B25" s="28">
-        <v>18</v>
-      </c>
-      <c r="C25" s="45"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="61"/>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="28">
-        <v>19</v>
-      </c>
-      <c r="C26" s="45"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="61"/>
+      <c r="C26" s="44"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="66"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B27" s="28">
+      <c r="B27" s="27">
         <v>20</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="61"/>
+      <c r="C27" s="44"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="66"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B28" s="28">
+      <c r="B28" s="27">
         <v>21</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="61"/>
+      <c r="C28" s="44"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="66"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B29" s="28">
+      <c r="B29" s="27">
         <v>22</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="61"/>
+      <c r="C29" s="44"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="66"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="28">
+      <c r="B30" s="27">
         <v>23</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="61"/>
+      <c r="C30" s="44"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="E31" s="59"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="61"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="66"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="E32" s="59"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="61"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="66"/>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E33" s="59"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="61"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="66"/>
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E34" s="59"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="61"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="66"/>
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E35" s="59"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="61"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
+      <c r="K35" s="66"/>
     </row>
     <row r="36" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E36" s="59"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="61"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="66"/>
     </row>
     <row r="37" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E37" s="59"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="60"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="61"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
+      <c r="K37" s="66"/>
     </row>
     <row r="38" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E38" s="62"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="63"/>
-      <c r="K38" s="64"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="68"/>
+      <c r="K38" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="N19:P19"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="M9:O9"/>
     <mergeCell ref="E9:K38"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="E5:K5"/>
@@ -3481,12 +3484,6 @@
     <mergeCell ref="N14:P14"/>
     <mergeCell ref="N18:P18"/>
     <mergeCell ref="N17:P17"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="N19:P19"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="M9:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3501,513 +3498,493 @@
   </sheetPr>
   <dimension ref="B1:Y20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="32"/>
-    <col min="2" max="2" width="16.109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" style="32" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="32" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" style="32" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36" style="32" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" style="32" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" style="32" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" style="32" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" style="32" customWidth="1"/>
-    <col min="13" max="13" width="20.77734375" style="32" customWidth="1"/>
-    <col min="14" max="14" width="30.5546875" style="32" customWidth="1"/>
-    <col min="15" max="15" width="7.5546875" style="32" customWidth="1"/>
-    <col min="16" max="16" width="8.5546875" style="32" customWidth="1"/>
-    <col min="17" max="18" width="9.109375" style="32"/>
-    <col min="19" max="19" width="2.5546875" style="32" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.44140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.44140625" style="32" customWidth="1"/>
-    <col min="23" max="23" width="2.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.21875" style="32" customWidth="1"/>
-    <col min="25" max="25" width="5.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="32"/>
+    <col min="1" max="1" width="9.109375" style="31"/>
+    <col min="2" max="2" width="16.109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="31" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" style="31" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="31" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36" style="31" customWidth="1"/>
+    <col min="8" max="8" width="22.44140625" style="31" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" style="31" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" style="31" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" style="31" customWidth="1"/>
+    <col min="14" max="14" width="30.5546875" style="31" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" style="31" customWidth="1"/>
+    <col min="16" max="16" width="8.5546875" style="31" customWidth="1"/>
+    <col min="17" max="18" width="9.109375" style="31"/>
+    <col min="19" max="19" width="2.5546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.44140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.44140625" style="31" customWidth="1"/>
+    <col min="23" max="23" width="2.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.21875" style="31" customWidth="1"/>
+    <col min="25" max="25" width="5.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B1" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="60"/>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="I2" s="21" t="s">
-        <v>55</v>
+      <c r="I2" s="20" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="95" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="32"/>
+      <c r="L3" s="32"/>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="99"/>
+      <c r="R6" s="99"/>
+      <c r="S6" s="99"/>
+      <c r="T6" s="99"/>
+      <c r="U6" s="99"/>
+      <c r="V6" s="99"/>
+      <c r="W6" s="99"/>
+      <c r="X6" s="99"/>
+      <c r="Y6" s="99"/>
+    </row>
+    <row r="7" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="99"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="103" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="104" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="104"/>
+      <c r="Q7" s="104"/>
+      <c r="R7" s="104"/>
+      <c r="S7" s="105" t="s">
+        <v>77</v>
+      </c>
+      <c r="T7" s="105"/>
+      <c r="U7" s="105"/>
+      <c r="V7" s="105"/>
+      <c r="W7" s="105"/>
+      <c r="X7" s="105"/>
+      <c r="Y7" s="105"/>
+    </row>
+    <row r="8" spans="2:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="99"/>
+      <c r="C8" s="80" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="33"/>
-      <c r="L3" s="33"/>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="32"/>
-    </row>
-    <row r="6" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="71" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="114" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="72" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="71"/>
-      <c r="U6" s="71"/>
-      <c r="V6" s="71"/>
-      <c r="W6" s="71"/>
-      <c r="X6" s="71"/>
-      <c r="Y6" s="71"/>
-    </row>
-    <row r="7" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="109" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="75"/>
-      <c r="S7" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="T7" s="76"/>
-      <c r="U7" s="76"/>
-      <c r="V7" s="76"/>
-      <c r="W7" s="76"/>
-      <c r="X7" s="76"/>
-      <c r="Y7" s="76"/>
-    </row>
-    <row r="8" spans="2:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="71"/>
-      <c r="C8" s="72" t="s">
+      <c r="E8" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="72" t="s">
+      <c r="F8" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="77" t="s">
+      <c r="G8" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="101"/>
+      <c r="I8" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="83"/>
+      <c r="K8" s="82" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" s="83"/>
+      <c r="M8" s="82" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="83"/>
+      <c r="O8" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" s="86" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="86" t="s">
+        <v>69</v>
+      </c>
+      <c r="R8" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="S8" s="88">
+        <v>0</v>
+      </c>
+      <c r="T8" s="88">
+        <v>1</v>
+      </c>
+      <c r="U8" s="88">
+        <v>2</v>
+      </c>
+      <c r="V8" s="88" t="s">
+        <v>23</v>
+      </c>
+      <c r="W8" s="88" t="s">
+        <v>24</v>
+      </c>
+      <c r="X8" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y8" s="88" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="99"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="87"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="87"/>
+      <c r="R9" s="87"/>
+      <c r="S9" s="89"/>
+      <c r="T9" s="89"/>
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+      <c r="X9" s="89"/>
+      <c r="Y9" s="89"/>
+    </row>
+    <row r="10" spans="2:25" ht="78" x14ac:dyDescent="0.3">
+      <c r="B10" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="77" t="s">
+      <c r="D10" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="110"/>
-      <c r="I8" s="107" t="s">
-        <v>75</v>
-      </c>
-      <c r="J8" s="108"/>
-      <c r="K8" s="107" t="s">
-        <v>76</v>
-      </c>
-      <c r="L8" s="108"/>
-      <c r="M8" s="107" t="s">
-        <v>77</v>
-      </c>
-      <c r="N8" s="108"/>
-      <c r="O8" s="103" t="s">
-        <v>48</v>
-      </c>
-      <c r="P8" s="103" t="s">
+      <c r="J10" s="38"/>
+      <c r="K10" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="L10" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="M10" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="N10" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="O10" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="P10" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q10" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="R10" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="X10" s="40"/>
+      <c r="Y10" s="40"/>
+    </row>
+    <row r="11" spans="2:25" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="35"/>
+      <c r="G11" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="T11" s="40"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="40"/>
+      <c r="W11" s="40"/>
+      <c r="X11" s="40"/>
+      <c r="Y11" s="40"/>
+    </row>
+    <row r="12" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="40"/>
+      <c r="X12" s="40"/>
+      <c r="Y12" s="40"/>
+    </row>
+    <row r="13" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="40"/>
+      <c r="Y13" s="40"/>
+    </row>
+    <row r="14" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="40"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="F15" s="31"/>
+    </row>
+    <row r="16" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="94"/>
+      <c r="N18" s="94"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="Q8" s="103" t="s">
-        <v>70</v>
-      </c>
-      <c r="R8" s="103" t="s">
-        <v>71</v>
-      </c>
-      <c r="S8" s="105">
-        <v>0</v>
-      </c>
-      <c r="T8" s="105">
-        <v>1</v>
-      </c>
-      <c r="U8" s="105">
-        <v>2</v>
-      </c>
-      <c r="V8" s="105" t="s">
-        <v>23</v>
-      </c>
-      <c r="W8" s="105" t="s">
-        <v>24</v>
-      </c>
-      <c r="X8" s="105" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y8" s="105" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="71"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" s="104"/>
-      <c r="P9" s="104"/>
-      <c r="Q9" s="104"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="106"/>
-      <c r="W9" s="106"/>
-      <c r="X9" s="106"/>
-      <c r="Y9" s="106"/>
-    </row>
-    <row r="10" spans="2:25" ht="78" x14ac:dyDescent="0.3">
-      <c r="B10" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="113" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="36"/>
-      <c r="G10" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="I10" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="L10" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="M10" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="N10" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="O10" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="P10" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q10" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="R10" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="S10" s="41"/>
-      <c r="T10" s="41"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="41"/>
-      <c r="W10" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-    </row>
-    <row r="11" spans="2:25" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="113" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="121" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="40"/>
-      <c r="S11" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="T11" s="41"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="41"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-    </row>
-    <row r="12" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="40"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-    </row>
-    <row r="13" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="40"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="40"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-    </row>
-    <row r="14" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="F15" s="32"/>
-    </row>
-    <row r="16" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="32"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="80" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="80"/>
-      <c r="I18" s="80"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="80"/>
-      <c r="M18" s="80"/>
-      <c r="N18" s="80"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="83" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="83"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="83"/>
-      <c r="K19" s="83"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="83"/>
-      <c r="N19" s="83"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="92"/>
+      <c r="J19" s="92"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="92"/>
+      <c r="M19" s="92"/>
+      <c r="N19" s="92"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="81" t="s">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="82"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="82"/>
-      <c r="M20" s="82"/>
-      <c r="N20" s="82"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="91"/>
+      <c r="M20" s="91"/>
+      <c r="N20" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C6:F7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="G20:N20"/>
-    <mergeCell ref="G19:N19"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="G18:N18"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B6:B9"/>
@@ -4021,6 +3998,26 @@
     <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="W8:W9"/>
     <mergeCell ref="X8:X9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="G20:N20"/>
+    <mergeCell ref="G19:N19"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="G18:N18"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="I8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4033,10 +4030,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:R15"/>
+  <dimension ref="B1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:Q5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4054,92 +4051,63 @@
     <col min="13" max="13" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="54"/>
-    </row>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="84" t="s">
+      <c r="G1" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="60"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="L3" s="86" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="133"/>
-      <c r="P3" s="134"/>
-      <c r="Q3" s="89" t="s">
-        <v>54</v>
-      </c>
-      <c r="R3" s="92" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="127" t="s">
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+    </row>
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="122" t="s">
+      <c r="D4" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="96" t="s">
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="97"/>
-      <c r="L4" s="126" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="125" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="125" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="135" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" s="136"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="93"/>
-    </row>
-    <row r="5" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="128"/>
-      <c r="C5" s="99"/>
+      <c r="I4" s="129"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="113"/>
+      <c r="C5" s="111"/>
       <c r="D5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>4</v>
@@ -4147,76 +4115,56 @@
       <c r="I5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="95"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="131"/>
-      <c r="P5" s="132"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="94"/>
-    </row>
-    <row r="6" spans="2:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:10" ht="44.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="36" t="s">
+      <c r="C6" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="120" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="113" t="s">
-        <v>93</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37" t="s">
+      <c r="F6" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="134" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="L6" s="14">
-        <v>2</v>
-      </c>
-      <c r="M6" s="15">
-        <v>1</v>
-      </c>
-      <c r="N6" s="15">
-        <v>1</v>
-      </c>
-      <c r="O6" s="129" t="s">
-        <v>41</v>
-      </c>
-      <c r="P6" s="130"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="17"/>
-    </row>
-    <row r="7" spans="2:18" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>2</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="36" t="s">
+      <c r="C7" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="113" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="121" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I7" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4224,31 +4172,31 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="2:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -4259,39 +4207,97 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
       <c r="G12" s="9"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I13" s="2"/>
     </row>
-    <row r="15" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="132" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="133"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="106"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="120" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="123" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="14.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="108" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="108" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="116" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="117"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="124"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="127"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="122"/>
+      <c r="H16" s="125"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="45">
+        <v>2</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1</v>
+      </c>
+      <c r="E17" s="114">
+        <f>16*100/16</f>
+        <v>100</v>
+      </c>
+      <c r="F17" s="115"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="G1:J1"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="O4:P5"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="R3:R5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="L3:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4305,15 +4311,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A33786056CB34C49BCEFA0219ACF09AA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="85f5b5ac1e835e7529ebd9eccdd2982d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="63f82232-4b4a-4992-a008-0c2680091aa8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585b424e621faf372cd06dff5902e016" ns2:_="">
     <xsd:import namespace="63f82232-4b4a-4992-a008-0c2680091aa8"/>
@@ -4485,6 +4482,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{944387EB-9B1B-4756-9CBE-55FEEBFE0742}">
   <ds:schemaRefs>
@@ -4495,14 +4501,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A361FD91-AF80-44D8-88BD-DF90646571F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0411A5A1-1C19-4FB0-8B04-8DFF57B89C71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4518,4 +4516,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A361FD91-AF80-44D8-88BD-DF90646571F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify excel file, add CFG image.
</commit_message>
<xml_diff>
--- a/Docs/Lab4/Lab04_WBT_TCs_Form.xlsx
+++ b/Docs/Lab4/Lab04_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2B56C9-37F9-4A3A-827F-EEC9EBE8BA81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239C2BB0-9577-44C5-AD75-4FF246EBA947}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cerinta" sheetId="1" r:id="rId1"/>
@@ -1243,6 +1243,9 @@
     <xf numFmtId="49" fontId="18" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1270,6 +1273,12 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1300,15 +1309,87 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1327,83 +1408,32 @@
     <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1411,12 +1441,48 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1428,72 +1494,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2105,22 +2105,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>105450</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3630120</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>3390900</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>14174</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9293099-0792-4726-814D-4BC702D8C277}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61EFFCAE-8754-43FB-8D0B-8CC97EC4BB0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2142,8 +2142,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6431280" y="1882140"/>
-          <a:ext cx="7219140" cy="4594860"/>
+          <a:off x="6468150" y="1737360"/>
+          <a:ext cx="6943050" cy="5043374"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2155,22 +2155,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="TextBox 3">
+        <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD6122A8-EEA7-49D4-A7B7-9F090013CE17}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40140FC3-3E97-445E-8AFB-C187AA5D09D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2178,8 +2178,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10332720" y="4335780"/>
-          <a:ext cx="259080" cy="243840"/>
+          <a:off x="10454640" y="3741420"/>
+          <a:ext cx="251460" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2215,8 +2215,11 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2</a:t>
-          </a:r>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2224,23 +2227,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5">
+        <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4D63DA7-2C29-4912-B646-7F0243FD4340}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA89DED-221F-4491-A8A1-0581EE55B523}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2248,8 +2251,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9083040" y="5600700"/>
-          <a:ext cx="228600" cy="243840"/>
+          <a:off x="7520940" y="4541520"/>
+          <a:ext cx="251460" cy="243840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2285,7 +2288,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1</a:t>
+            <a:t>2</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2294,23 +2297,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1592580</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1882140</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextBox 6">
+        <xdr:cNvPr id="12" name="TextBox 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EBECFB4-FB73-45A4-B243-AEFBAA183067}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8BE1D92-A964-4FCC-8855-6B4483A2722E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2318,8 +2321,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11612880" y="3360420"/>
-          <a:ext cx="289560" cy="304800"/>
+          <a:off x="8846820" y="5433060"/>
+          <a:ext cx="274320" cy="236220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2356,6 +2359,76 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1844040</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{931E2F04-4832-4BE7-83F6-63E9ABD0F988}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11864340" y="2872740"/>
+          <a:ext cx="289560" cy="259080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>4</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2816,12 +2889,12 @@
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B1" s="12"/>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="L2" s="13" t="s">
@@ -2832,33 +2905,33 @@
       <c r="O2" s="13"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="L3" s="52" t="s">
+      <c r="L3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="54" t="s">
+      <c r="M3" s="54"/>
+      <c r="N3" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="57"/>
     </row>
     <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="L4" s="57" t="s">
+      <c r="L4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="57"/>
+      <c r="M4" s="58"/>
       <c r="N4" s="19" t="s">
         <v>57</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="54">
+      <c r="P4" s="55">
         <v>1211</v>
       </c>
-      <c r="Q4" s="56"/>
+      <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -2927,8 +3000,8 @@
   </sheetPr>
   <dimension ref="B1:P38"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2947,34 +3020,34 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="22"/>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="60"/>
+      <c r="D1" s="61"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C2" s="24"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="E5" s="58" t="s">
+      <c r="C5" s="60"/>
+      <c r="E5" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="M5" s="70" t="s">
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="M5" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
@@ -2986,13 +3059,13 @@
       <c r="E7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="72" t="s">
+      <c r="M7" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
       <c r="P7" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -3005,12 +3078,12 @@
       <c r="E8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="72" t="s">
+      <c r="M8" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="26">
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="48">
         <f>8-7+2</f>
         <v>3</v>
       </c>
@@ -3022,21 +3095,21 @@
       <c r="C9" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="61"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="63"/>
-      <c r="M9" s="72" t="s">
+      <c r="E9" s="64"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="66"/>
+      <c r="M9" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="72" t="s">
+      <c r="N9" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="72"/>
-      <c r="P9" s="48">
+      <c r="O9" s="63"/>
+      <c r="P9">
         <f>3+1</f>
         <v>4</v>
       </c>
@@ -3048,13 +3121,13 @@
       <c r="C10" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="64"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="69"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="27">
@@ -3063,13 +3136,13 @@
       <c r="C11" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="64"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="66"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="69"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="27">
@@ -3078,19 +3151,19 @@
       <c r="C12" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="66"/>
-      <c r="M12" s="70" t="s">
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="69"/>
+      <c r="M12" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="N12" s="70"/>
-      <c r="O12" s="70"/>
-      <c r="P12" s="70"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="27">
@@ -3099,13 +3172,13 @@
       <c r="C13" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="64"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
-      <c r="K13" s="66"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="69"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="27">
@@ -3114,21 +3187,21 @@
       <c r="C14" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="64"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="K14" s="66"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="69"/>
       <c r="M14" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="73" t="s">
+      <c r="N14" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
+      <c r="O14" s="74"/>
+      <c r="P14" s="74"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="27">
@@ -3137,21 +3210,21 @@
       <c r="C15" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="66"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="69"/>
       <c r="M15" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="N15" s="71" t="s">
+      <c r="N15" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="O15" s="71"/>
-      <c r="P15" s="71"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="27">
@@ -3160,21 +3233,21 @@
       <c r="C16" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="64"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="69"/>
       <c r="M16" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="N16" s="71" t="s">
+      <c r="N16" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="O16" s="71"/>
-      <c r="P16" s="71"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="62"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="27">
@@ -3183,289 +3256,291 @@
       <c r="C17" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="64"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="66"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="69"/>
       <c r="M17" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="N17" s="71" t="s">
+      <c r="N17" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="O17" s="71"/>
-      <c r="P17" s="71"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="62"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="27">
         <v>11</v>
       </c>
       <c r="C18" s="44"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="66"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="69"/>
       <c r="M18" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="N18" s="71" t="s">
+      <c r="N18" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="O18" s="71"/>
-      <c r="P18" s="71"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="62"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="27">
         <v>12</v>
       </c>
       <c r="C19" s="44"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="66"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="69"/>
       <c r="M19" s="21"/>
-      <c r="N19" s="71"/>
-      <c r="O19" s="71"/>
-      <c r="P19" s="71"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="27">
         <v>13</v>
       </c>
       <c r="C20" s="44"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="69"/>
       <c r="M20" s="29"/>
-      <c r="N20" s="71"/>
-      <c r="O20" s="71"/>
-      <c r="P20" s="71"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
+      <c r="P20" s="62"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="27">
         <v>14</v>
       </c>
       <c r="C21" s="44"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="66"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="69"/>
       <c r="M21" s="21"/>
-      <c r="N21" s="71"/>
-      <c r="O21" s="71"/>
-      <c r="P21" s="71"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="62"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="27">
         <v>15</v>
       </c>
       <c r="C22" s="44"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="66"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="69"/>
       <c r="M22" s="21"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="71"/>
-      <c r="P22" s="71"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="62"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="27">
         <v>16</v>
       </c>
       <c r="C23" s="44"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="66"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="27">
         <v>17</v>
       </c>
       <c r="C24" s="44"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="66"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="69"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="27">
         <v>18</v>
       </c>
       <c r="C25" s="44"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="65"/>
-      <c r="K25" s="66"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="27">
         <v>19</v>
       </c>
       <c r="C26" s="44"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
-      <c r="K26" s="66"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="69"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="27">
         <v>20</v>
       </c>
       <c r="C27" s="44"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="66"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="27">
         <v>21</v>
       </c>
       <c r="C28" s="44"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="66"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="69"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="27">
         <v>22</v>
       </c>
       <c r="C29" s="44"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="66"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="69"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="27">
         <v>23</v>
       </c>
       <c r="C30" s="44"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="66"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="69"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="E31" s="64"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="66"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="69"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="E32" s="64"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="66"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="69"/>
     </row>
     <row r="33" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E33" s="64"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="65"/>
-      <c r="K33" s="66"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="69"/>
     </row>
     <row r="34" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E34" s="64"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="66"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="69"/>
     </row>
     <row r="35" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E35" s="64"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="66"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="69"/>
     </row>
     <row r="36" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E36" s="64"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="66"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="68"/>
+      <c r="K36" s="69"/>
     </row>
     <row r="37" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E37" s="64"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="K37" s="66"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="68"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="69"/>
     </row>
     <row r="38" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E38" s="67"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="69"/>
+      <c r="E38" s="70"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N17:P17"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="N21:P21"/>
     <mergeCell ref="N22:P22"/>
@@ -3482,8 +3557,6 @@
     <mergeCell ref="M12:P12"/>
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N17:P17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3498,7 +3571,7 @@
   </sheetPr>
   <dimension ref="B1:Y20"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3532,15 +3605,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="61"/>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.3">
       <c r="I2" s="20" t="s">
@@ -3548,16 +3621,16 @@
       </c>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="98"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="78"/>
       <c r="J3" s="32"/>
       <c r="L3" s="32"/>
     </row>
@@ -3569,75 +3642,75 @@
       <c r="F5" s="31"/>
     </row>
     <row r="6" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="76"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="103"/>
       <c r="G6" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="99" t="s">
+      <c r="H6" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="99"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="99"/>
-      <c r="N6" s="99"/>
-      <c r="O6" s="99"/>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="99"/>
-      <c r="S6" s="99"/>
-      <c r="T6" s="99"/>
-      <c r="U6" s="99"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="99"/>
-      <c r="X6" s="99"/>
-      <c r="Y6" s="99"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="79"/>
+      <c r="Q6" s="79"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="79"/>
+      <c r="U6" s="79"/>
+      <c r="V6" s="79"/>
+      <c r="W6" s="79"/>
+      <c r="X6" s="79"/>
+      <c r="Y6" s="79"/>
     </row>
     <row r="7" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="99"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="106"/>
       <c r="G7" s="81"/>
-      <c r="H7" s="100" t="s">
+      <c r="H7" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="103" t="s">
+      <c r="I7" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103"/>
-      <c r="N7" s="103"/>
-      <c r="O7" s="104" t="s">
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="P7" s="104"/>
-      <c r="Q7" s="104"/>
-      <c r="R7" s="104"/>
-      <c r="S7" s="105" t="s">
+      <c r="P7" s="86"/>
+      <c r="Q7" s="86"/>
+      <c r="R7" s="86"/>
+      <c r="S7" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="T7" s="105"/>
-      <c r="U7" s="105"/>
-      <c r="V7" s="105"/>
-      <c r="W7" s="105"/>
-      <c r="X7" s="105"/>
-      <c r="Y7" s="105"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="87"/>
     </row>
     <row r="8" spans="2:25" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="99"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="80" t="s">
         <v>80</v>
       </c>
@@ -3647,67 +3720,67 @@
       <c r="E8" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="88" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="84" t="s">
+      <c r="G8" s="88" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="101"/>
-      <c r="I8" s="82" t="s">
+      <c r="H8" s="83"/>
+      <c r="I8" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="J8" s="83"/>
-      <c r="K8" s="82" t="s">
+      <c r="J8" s="100"/>
+      <c r="K8" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="L8" s="83"/>
-      <c r="M8" s="82" t="s">
+      <c r="L8" s="100"/>
+      <c r="M8" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="N8" s="83"/>
-      <c r="O8" s="86" t="s">
+      <c r="N8" s="100"/>
+      <c r="O8" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="86" t="s">
+      <c r="P8" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="Q8" s="86" t="s">
+      <c r="Q8" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="R8" s="86" t="s">
+      <c r="R8" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="S8" s="88">
+      <c r="S8" s="90">
         <v>0</v>
       </c>
-      <c r="T8" s="88">
+      <c r="T8" s="90">
         <v>1</v>
       </c>
-      <c r="U8" s="88">
+      <c r="U8" s="90">
         <v>2</v>
       </c>
-      <c r="V8" s="88" t="s">
+      <c r="V8" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="W8" s="88" t="s">
+      <c r="W8" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="X8" s="88" t="s">
+      <c r="X8" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="Y8" s="88" t="s">
+      <c r="Y8" s="90" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:25" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="99"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="81"/>
       <c r="D9" s="81"/>
       <c r="E9" s="81"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="102"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="84"/>
       <c r="I9" s="34" t="s">
         <v>27</v>
       </c>
@@ -3726,17 +3799,17 @@
       <c r="N9" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="87"/>
-      <c r="P9" s="87"/>
-      <c r="Q9" s="87"/>
-      <c r="R9" s="87"/>
-      <c r="S9" s="89"/>
-      <c r="T9" s="89"/>
-      <c r="U9" s="89"/>
-      <c r="V9" s="89"/>
-      <c r="W9" s="89"/>
-      <c r="X9" s="89"/>
-      <c r="Y9" s="89"/>
+      <c r="O9" s="93"/>
+      <c r="P9" s="93"/>
+      <c r="Q9" s="93"/>
+      <c r="R9" s="93"/>
+      <c r="S9" s="91"/>
+      <c r="T9" s="91"/>
+      <c r="U9" s="91"/>
+      <c r="V9" s="91"/>
+      <c r="W9" s="91"/>
+      <c r="X9" s="91"/>
+      <c r="Y9" s="91"/>
     </row>
     <row r="10" spans="2:25" ht="78" x14ac:dyDescent="0.3">
       <c r="B10" s="35" t="s">
@@ -3931,23 +4004,23 @@
       <c r="F16" s="31"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="94" t="s">
+      <c r="C18" s="97"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="94"/>
-      <c r="I18" s="94"/>
-      <c r="J18" s="94"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="94"/>
-      <c r="N18" s="94"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="98"/>
+      <c r="L18" s="98"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="98"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="42"/>
@@ -3955,16 +4028,16 @@
       <c r="D19" s="42"/>
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
-      <c r="G19" s="92" t="s">
+      <c r="G19" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="H19" s="92"/>
-      <c r="I19" s="92"/>
-      <c r="J19" s="92"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="92"/>
-      <c r="M19" s="92"/>
-      <c r="N19" s="92"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="96"/>
+      <c r="J19" s="96"/>
+      <c r="K19" s="96"/>
+      <c r="L19" s="96"/>
+      <c r="M19" s="96"/>
+      <c r="N19" s="96"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="42"/>
@@ -3972,19 +4045,36 @@
       <c r="D20" s="42"/>
       <c r="E20" s="42"/>
       <c r="F20" s="42"/>
-      <c r="G20" s="90" t="s">
+      <c r="G20" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="91"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="95"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G20:N20"/>
+    <mergeCell ref="G19:N19"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="G18:N18"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="B6:B9"/>
@@ -3999,25 +4089,8 @@
     <mergeCell ref="W8:W9"/>
     <mergeCell ref="X8:X9"/>
     <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="G20:N20"/>
-    <mergeCell ref="G19:N19"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="G18:N18"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="O8:O9"/>
     <mergeCell ref="C6:F7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="I8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4032,7 +4105,7 @@
   </sheetPr>
   <dimension ref="B1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -4057,46 +4130,46 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="130" t="s">
+      <c r="B3" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="131"/>
-      <c r="D3" s="131"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="131"/>
-      <c r="I3" s="131"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="134" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="110" t="s">
+      <c r="C4" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="128" t="s">
+      <c r="D4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="129"/>
-      <c r="H4" s="128" t="s">
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="129"/>
+      <c r="I4" s="111"/>
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="113"/>
-      <c r="C5" s="111"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="133"/>
       <c r="D5" s="7" t="s">
         <v>80</v>
       </c>
@@ -4136,7 +4209,7 @@
       <c r="H6" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="I6" s="134" t="s">
+      <c r="I6" s="52" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4223,45 +4296,45 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="132" t="s">
+      <c r="B14" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="120" t="s">
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="117"/>
+      <c r="G14" s="118" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="123" t="s">
+      <c r="H14" s="121" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="14.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="126" t="s">
+      <c r="B15" s="124" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="108" t="s">
+      <c r="D15" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="116" t="s">
+      <c r="E15" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="117"/>
-      <c r="G15" s="121"/>
-      <c r="H15" s="124"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="122"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="127"/>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="119"/>
-      <c r="G16" s="122"/>
-      <c r="H16" s="125"/>
+      <c r="B16" s="125"/>
+      <c r="C16" s="127"/>
+      <c r="D16" s="127"/>
+      <c r="E16" s="130"/>
+      <c r="F16" s="131"/>
+      <c r="G16" s="120"/>
+      <c r="H16" s="123"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="45">
@@ -4273,16 +4346,19 @@
       <c r="D17" s="14">
         <v>1</v>
       </c>
-      <c r="E17" s="114">
+      <c r="E17" s="107">
         <f>16*100/16</f>
         <v>100</v>
       </c>
-      <c r="F17" s="115"/>
+      <c r="F17" s="108"/>
       <c r="G17" s="15"/>
       <c r="H17" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="H4:I4"/>
@@ -4295,9 +4371,6 @@
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="E15:F16"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4311,6 +4384,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A33786056CB34C49BCEFA0219ACF09AA" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="85f5b5ac1e835e7529ebd9eccdd2982d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="63f82232-4b4a-4992-a008-0c2680091aa8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585b424e621faf372cd06dff5902e016" ns2:_="">
     <xsd:import namespace="63f82232-4b4a-4992-a008-0c2680091aa8"/>
@@ -4482,15 +4564,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{944387EB-9B1B-4756-9CBE-55FEEBFE0742}">
   <ds:schemaRefs>
@@ -4501,6 +4574,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A361FD91-AF80-44D8-88BD-DF90646571F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0411A5A1-1C19-4FB0-8B04-8DFF57B89C71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4516,12 +4597,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A361FD91-AF80-44D8-88BD-DF90646571F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>